<commit_message>
TestTask.Test: Add CategoryImortTest and Change one resources file.
</commit_message>
<xml_diff>
--- a/TestTask.Test/Resources/NotCorrectDataIsAllFilledIn.xlsx
+++ b/TestTask.Test/Resources/NotCorrectDataIsAllFilledIn.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\TASK\TestTask.Data\22.11.2023_22-45\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\TestTask\TestTask.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF72CDF-3EFB-4FE8-B302-462AACD85A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC9E134-AB3B-41F4-80DB-1D4B159A1B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Rick&amp;Morty</t>
-  </si>
-  <si>
-    <t>Clothe</t>
   </si>
   <si>
     <t>Electronic</t>
@@ -562,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -597,7 +594,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -613,16 +612,13 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -634,7 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -661,10 +657,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -675,12 +671,12 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>2</v>

</xml_diff>

<commit_message>
TestTask - Change type ID (int -> Guid). Change methods solution for ID.
</commit_message>
<xml_diff>
--- a/TestTask.Test/Resources/NotCorrectDataIsAllFilledIn.xlsx
+++ b/TestTask.Test/Resources/NotCorrectDataIsAllFilledIn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\TestTask\TestTask.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD0EDD0-0BDB-4370-9EAC-2D715591BA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF251F9-1E47-4EA3-828B-E2934AEA2115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2190" yWindow="2220" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -86,6 +86,33 @@
   </si>
   <si>
     <t>NOT</t>
+  </si>
+  <si>
+    <t>4af33f61-8fe2-461b-8eae-cc8344feebe8</t>
+  </si>
+  <si>
+    <t>ff1c323c-123b-4eb4-b3cd-1884bd053b07</t>
+  </si>
+  <si>
+    <t>54d22ad6-5748-4ea7-b7e9-c7a4e0b52220</t>
+  </si>
+  <si>
+    <t>6ae9a401-0a41-4384-8f36-4b67df9846d1</t>
+  </si>
+  <si>
+    <t>36e632d2-98b2-4a1b-8c8f-268aac79271e</t>
+  </si>
+  <si>
+    <t>54d32ad6-5748-4ea7-b7e9-c7a4e0b52220</t>
+  </si>
+  <si>
+    <t>c0606848-ba9a-41fd-bdf2-d355188803eb</t>
+  </si>
+  <si>
+    <t>a00ad315-a4a9-406c-9cb4-b15487b016a9</t>
+  </si>
+  <si>
+    <t>c5506848-ba9a-41fd-bdf2-d355188803eb</t>
   </si>
 </sst>
 </file>
@@ -121,8 +148,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -440,7 +469,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,8 +489,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -471,8 +500,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -493,11 +522,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -523,17 +559,18 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="F2">
         <v>235</v>
@@ -543,20 +580,20 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -566,17 +603,18 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F4">
         <v>400</v>
@@ -587,6 +625,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -594,11 +633,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -609,8 +652,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -630,11 +673,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -648,11 +695,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,13 +709,13 @@
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -678,16 +725,16 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
-        <v>2</v>
+      <c r="C5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change type ID (int -> Guid) (#138)
* TestTask - Change type ID (int -> Guid). Change methods solution for ID.

* TestTask.Migration - Add migration in DB.
</commit_message>
<xml_diff>
--- a/TestTask.Test/Resources/NotCorrectDataIsAllFilledIn.xlsx
+++ b/TestTask.Test/Resources/NotCorrectDataIsAllFilledIn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\TestTask\TestTask.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD0EDD0-0BDB-4370-9EAC-2D715591BA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF251F9-1E47-4EA3-828B-E2934AEA2115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2190" yWindow="2220" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -86,6 +86,33 @@
   </si>
   <si>
     <t>NOT</t>
+  </si>
+  <si>
+    <t>4af33f61-8fe2-461b-8eae-cc8344feebe8</t>
+  </si>
+  <si>
+    <t>ff1c323c-123b-4eb4-b3cd-1884bd053b07</t>
+  </si>
+  <si>
+    <t>54d22ad6-5748-4ea7-b7e9-c7a4e0b52220</t>
+  </si>
+  <si>
+    <t>6ae9a401-0a41-4384-8f36-4b67df9846d1</t>
+  </si>
+  <si>
+    <t>36e632d2-98b2-4a1b-8c8f-268aac79271e</t>
+  </si>
+  <si>
+    <t>54d32ad6-5748-4ea7-b7e9-c7a4e0b52220</t>
+  </si>
+  <si>
+    <t>c0606848-ba9a-41fd-bdf2-d355188803eb</t>
+  </si>
+  <si>
+    <t>a00ad315-a4a9-406c-9cb4-b15487b016a9</t>
+  </si>
+  <si>
+    <t>c5506848-ba9a-41fd-bdf2-d355188803eb</t>
   </si>
 </sst>
 </file>
@@ -121,8 +148,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -440,7 +469,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,8 +489,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -471,8 +500,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -493,11 +522,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -523,17 +559,18 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="F2">
         <v>235</v>
@@ -543,20 +580,20 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -566,17 +603,18 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F4">
         <v>400</v>
@@ -587,6 +625,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -594,11 +633,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -609,8 +652,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -630,11 +673,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -648,11 +695,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,13 +709,13 @@
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -678,16 +725,16 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
-        <v>2</v>
+      <c r="C5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>